<commit_message>
keep last 2 unquerieable have zero RID rows
</commit_message>
<xml_diff>
--- a/keep.xlsx
+++ b/keep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-snowflake/snowflake-connector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F393609E-5741-FB46-B3BF-A27CF5930A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{7C960CAC-F71A-574C-8BB7-17993D161508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53700" yWindow="8060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
   <si>
     <t>metadata_table</t>
   </si>
@@ -357,70 +357,28 @@
     <t>{'SEGMENT__ANGEL_FUNDING_PROD__IDENTIFIES@USER_ID_UUID-USERNAME_UUID-PERSONA_UUID': 110</t>
   </si>
   <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-USERNAME_UUID': 14093</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-PERSONA_UUID': 14661</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-RID_UUID': '0</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USERNAME_UUID-PERSONA_UUID': 13288</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USERNAME_UUID-RID_UUID': '0</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@PERSONA_UUID-RID_UUID': 0</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-USERNAME_UUID-PERSONA_UUID': 13288</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-USERNAME_UUID-RID_UUID': 0</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-PERSONA_UUID-RID_UUID': 0</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USERNAME_UUID-PERSONA_UUID-RID_UUID': 0</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-USERNAME_UUID-PERSONA_UUID-RID_UUID': 0</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-USERNAME_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USER_ID_UUID = USERNAME_UUID and USER_ID_UUID is not null and USERNAME_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-PERSONA_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USER_ID_UUID = PERSONA_UUID and USER_ID_UUID is not null and PERSONA_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-RID_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USER_ID_UUID = RID_UUID and USER_ID_UUID is not null and RID_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USERNAME_UUID-PERSONA_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USERNAME_UUID = PERSONA_UUID and USERNAME_UUID is not null and PERSONA_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USERNAME_UUID-RID_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USERNAME_UUID = RID_UUID and USERNAME_UUID is not null and RID_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@PERSONA_UUID-RID_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where PERSONA_UUID = RID_UUID and PERSONA_UUID is not null and RID_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-USERNAME_UUID-PERSONA_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USER_ID_UUID = USERNAME_UUID and USER_ID_UUID = PERSONA_UUID and USER_ID_UUID is not null and USERNAME_UUID is not null and PERSONA_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-USERNAME_UUID-RID_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USER_ID_UUID = USERNAME_UUID and USER_ID_UUID = RID_UUID and USER_ID_UUID is not null and USERNAME_UUID is not null and RID_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-PERSONA_UUID-RID_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USER_ID_UUID = PERSONA_UUID and USER_ID_UUID = RID_UUID and USER_ID_UUID is not null and PERSONA_UUID is not null and RID_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USERNAME_UUID-PERSONA_UUID-RID_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USERNAME_UUID = PERSONA_UUID and USERNAME_UUID = RID_UUID and USERNAME_UUID is not null and PERSONA_UUID is not null and RID_UUID is not null'}</t>
-  </si>
-  <si>
-    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-USERNAME_UUID-PERSONA_UUID-RID_UUID': 'SELECT count(*) from SEGMENT.IDENTIFIES_METADATA.SEGMENT__ANGEL_WEB__IDENTIFIES where USER_ID_UUID = USERNAME_UUID and USER_ID_UUID = PERSONA_UUID and USER_ID_UUID = RID_UUID and USER_ID_UUID is not null and USERNAME_UUID is not null and PERSONA_UUID is not null and RID_UUID is not null'}</t>
+    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-USERNAME_UUID: 14861</t>
+  </si>
+  <si>
+    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-PERSONA_UUID': 14665</t>
+  </si>
+  <si>
+    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USERNAME_UUID-PERSONA_UUID': 14053</t>
+  </si>
+  <si>
+    <t>{'SEGMENT__ANGEL_NFT_WEBSITE_PROD__IDENTIFIES@USER_ID_UUID-USERNAME_UUID-PERSONA_UUID': 14053</t>
+  </si>
+  <si>
+    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-USERNAME_UUID': 3955</t>
+  </si>
+  <si>
+    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-PERSONA_UUID': 21045</t>
+  </si>
+  <si>
+    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USERNAME_UUID-PERSONA_UUID': 2238</t>
+  </si>
+  <si>
+    <t>{'SEGMENT__ANGEL_WEB__IDENTIFIES@USER_ID_UUID-USERNAME_UUID-PERSONA_UUID': 2238</t>
   </si>
 </sst>
 </file>
@@ -1870,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2157,12 +2115,12 @@
     </row>
     <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D61" s="4" t="s">
@@ -2173,7 +2131,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="4" t="s">
         <v>108</v>
       </c>
       <c r="D62" s="4" t="s">
@@ -2184,243 +2142,160 @@
       </c>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="10"/>
+      <c r="F63" s="10">
+        <v>14665</v>
+      </c>
     </row>
     <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
+    </row>
+    <row r="65" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
+    <row r="73" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="67" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+    <row r="74" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+    <row r="75" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="69" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="76" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="4"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>62</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="97" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="98" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="99" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
+      <c r="A84" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" s="4" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" s="4" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>